<commit_message>
feat: Kleinuntehmerregelung nach §10 UStG einstellbar
</commit_message>
<xml_diff>
--- a/TestRechnung.xlsx
+++ b/TestRechnung.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herbe\Documents\Development\excel2zugferd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF6CD60-316D-48DA-B614-73F591FC99FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1E4DDE-5814-46EE-A1E4-940F172A0FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1920" windowWidth="30960" windowHeight="13992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2328" windowWidth="30960" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Rechnung2" sheetId="2" r:id="rId2"/>
+    <sheet name="Rechnung für Kleinunternehmen" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
   <si>
     <t>An:</t>
   </si>
@@ -67,49 +68,67 @@
     <t>h</t>
   </si>
   <si>
+    <t>Bruttobetrag</t>
+  </si>
+  <si>
+    <t>Kunde Hans Mustermann GmbH</t>
+  </si>
+  <si>
+    <t>Frau Mustermann</t>
+  </si>
+  <si>
+    <t>Musterstr. 10</t>
+  </si>
+  <si>
+    <t>12345 Musterstadt</t>
+  </si>
+  <si>
+    <t>WhatsApp wg. Netzteil für USB-Server</t>
+  </si>
+  <si>
+    <t>Telefonat wg. KVSiServer (steht in der Doku)</t>
+  </si>
+  <si>
+    <t>Bewerbungsgespräch mit Frau A und B</t>
+  </si>
+  <si>
+    <t>Email wg. Herrn R Anmeldung im AWS (hat versucht sich anzumelden mehr als 120 Tage vor Beginn der Reha, steht in der Logdatei im W2k19-fs)</t>
+  </si>
+  <si>
+    <t>Anmeldung im AWS von Patienten mit falscher MassnahmeID verbessert. Gemäß Email Fr. S.</t>
+  </si>
+  <si>
+    <t>Änderung Rehaziele im AWS und KVS-React gemäß Besprechung mit Frau S vom 01.12.2023</t>
+  </si>
+  <si>
+    <t>Email von Hrn F. bezüglich Anpassung Rechnungsnummern: An Herrn K verwiesen</t>
+  </si>
+  <si>
+    <t>Prüfung der Anmeldungen im AWS nach Email vom 17.01.2024 von Hrn. F</t>
+  </si>
+  <si>
+    <t>Email von Hrn. F bzgl. KVS Downtime und Funktion im Saal. (Kein KVS, keine Funktion im Saal)</t>
+  </si>
+  <si>
     <t>Umsatzsteuer 19%</t>
   </si>
   <si>
-    <t>Bruttobetrag</t>
-  </si>
-  <si>
-    <t>Kunde Hans Mustermann GmbH</t>
-  </si>
-  <si>
-    <t>Frau Mustermann</t>
-  </si>
-  <si>
-    <t>Musterstr. 10</t>
-  </si>
-  <si>
-    <t>12345 Musterstadt</t>
-  </si>
-  <si>
-    <t>WhatsApp wg. Netzteil für USB-Server</t>
-  </si>
-  <si>
-    <t>Telefonat wg. KVSiServer (steht in der Doku)</t>
-  </si>
-  <si>
-    <t>Bewerbungsgespräch mit Frau A und B</t>
-  </si>
-  <si>
-    <t>Email wg. Herrn R Anmeldung im AWS (hat versucht sich anzumelden mehr als 120 Tage vor Beginn der Reha, steht in der Logdatei im W2k19-fs)</t>
-  </si>
-  <si>
-    <t>Anmeldung im AWS von Patienten mit falscher MassnahmeID verbessert. Gemäß Email Fr. S.</t>
-  </si>
-  <si>
-    <t>Änderung Rehaziele im AWS und KVS-React gemäß Besprechung mit Frau S vom 01.12.2023</t>
-  </si>
-  <si>
-    <t>Email von Hrn F. bezüglich Anpassung Rechnungsnummern: An Herrn K verwiesen</t>
-  </si>
-  <si>
-    <t>Prüfung der Anmeldungen im AWS nach Email vom 17.01.2024 von Hrn. F</t>
-  </si>
-  <si>
-    <t>Email von Hrn. F bzgl. KVS Downtime und Funktion im Saal. (Kein KVS, keine Funktion im Saal)</t>
+    <t>Die Summe der Nettopreise, es wird in Spalte F nach "Summe" gesucht, bis zur nächsten Leerzeile</t>
+  </si>
+  <si>
+    <t>Die  Summe * 19%, oder 0 bei angewandter Kleinunternehmerregelung; es wird nach "Umsatzsteuer 19%" gesucht</t>
+  </si>
+  <si>
+    <t>Die Summe aus Summe + Umsatzsteuer; es wird nach "Bruttobetrag" gesucht</t>
+  </si>
+  <si>
+    <t>Alles zwischen "An:" und der nächsten Leerzeile wird für den Rechnungsempfänger verwendet.</t>
+  </si>
+  <si>
+    <t>Diese Zahl muss fortlaufend sein und kennzeichnet die Rechnungsnummer; Es wird nach "Rechnungs-Nr:" gesucht</t>
+  </si>
+  <si>
+    <t>Das sind die verwendeten Rechnungspositionen bis zur nächsten Leerzeile. Es wird nach "Pos." gesucht und dann weiter aufgeteilt.</t>
   </si>
 </sst>
 </file>
@@ -119,7 +138,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,6 +160,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -176,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -209,6 +236,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -517,13 +548,90 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -534,8 +642,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,22 +663,22 @@
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -614,7 +722,7 @@
         <v>45292</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6">
         <v>1</v>
@@ -640,7 +748,7 @@
         <v>45293</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -666,7 +774,7 @@
         <v>45294</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="6">
         <v>1</v>
@@ -692,7 +800,7 @@
         <v>45294</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="6">
         <v>2</v>
@@ -718,7 +826,7 @@
         <v>45295</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="6">
         <v>1</v>
@@ -744,7 +852,7 @@
         <v>45296</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
@@ -770,7 +878,7 @@
         <v>45302</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="6">
         <v>7</v>
@@ -796,7 +904,7 @@
         <v>45302</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="6">
         <v>1</v>
@@ -822,7 +930,7 @@
         <v>45309</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" s="6">
         <v>1</v>
@@ -848,7 +956,7 @@
         <v>45309</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
@@ -932,7 +1040,7 @@
     </row>
     <row r="35" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F35" s="12" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G35" s="12">
         <f>G34*19%</f>
@@ -941,7 +1049,7 @@
     </row>
     <row r="36" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F36" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G36" s="12">
         <f>SUM(G34:G35)</f>
@@ -956,4 +1064,430 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F435B499-96C6-4725-AFFC-8DE837C76B55}">
+  <dimension ref="A1:G37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.5546875" style="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13">
+        <v>20240001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7">
+        <v>45292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" ref="F10:F19" si="0">IF(E10="10 Min.",22,75)</f>
+        <v>22</v>
+      </c>
+      <c r="G10" s="12">
+        <f t="shared" ref="G10:G19" si="1">D10*F10</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <f t="shared" ref="A11:A19" si="2">A10+1</f>
+        <v>2</v>
+      </c>
+      <c r="B11" s="7">
+        <v>45293</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G11" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="B12" s="7">
+        <v>45294</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G12" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="B13" s="7">
+        <v>45294</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G13" s="12">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="B14" s="7">
+        <v>45295</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G14" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="B15" s="7">
+        <v>45296</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="6">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G15" s="12">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="B16" s="7">
+        <v>45302</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="6">
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G16" s="12">
+        <f t="shared" si="1"/>
+        <v>525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B17" s="7">
+        <v>45302</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="6">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G17" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="B18" s="7">
+        <v>45309</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G18" s="12">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B19" s="7">
+        <v>45309</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="8"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="8"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="8"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="8"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="8"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="8"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="8"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="8"/>
+      <c r="F27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="8"/>
+      <c r="F28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="8"/>
+      <c r="F29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="8"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="8"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="8"/>
+      <c r="F32" s="12"/>
+    </row>
+    <row r="33" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="8"/>
+      <c r="F33" s="12"/>
+    </row>
+    <row r="34" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="12">
+        <f>SUM(G10:G26)</f>
+        <v>957</v>
+      </c>
+    </row>
+    <row r="35" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F35" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F36" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="12">
+        <f>SUM(G34:G35)</f>
+        <v>957</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="8"/>
+      <c r="F37" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: #18 fixed and BT-73, BT-74, BT-134, BT-135 added
</commit_message>
<xml_diff>
--- a/TestRechnung.xlsx
+++ b/TestRechnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herbe\Documents\Development\excel2zugferd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1E4DDE-5814-46EE-A1E4-940F172A0FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86400CEB-223D-4EB6-8303-DF45461313B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2328" windowWidth="30960" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="276" yWindow="1500" windowWidth="20436" windowHeight="13992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
   <si>
     <t>An:</t>
   </si>
@@ -129,14 +129,18 @@
   </si>
   <si>
     <t>Das sind die verwendeten Rechnungspositionen bis zur nächsten Leerzeile. Es wird nach "Pos." gesucht und dann weiter aufgeteilt.</t>
+  </si>
+  <si>
+    <t>Anfahrt dazu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -203,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -241,6 +245,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -550,7 +561,7 @@
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -642,8 +653,8 @@
   </sheetPr>
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:G36"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -731,11 +742,11 @@
         <v>9</v>
       </c>
       <c r="F10" s="12">
-        <f t="shared" ref="F10:F19" si="0">IF(E10="10 Min.",22,75)</f>
+        <f t="shared" ref="F10:F20" si="0">IF(E10="10 Min.",22,75)</f>
         <v>22</v>
       </c>
       <c r="G10" s="12">
-        <f t="shared" ref="G10:G19" si="1">D10*F10</f>
+        <f t="shared" ref="G10:G20" si="1">D10*F10</f>
         <v>22</v>
       </c>
     </row>
@@ -974,8 +985,26 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E20" s="8"/>
-      <c r="F20" s="12"/>
+      <c r="A20" s="3">
+        <v>11</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E21" s="8"/>
@@ -1035,25 +1064,25 @@
       </c>
       <c r="G34" s="12">
         <f>SUM(G10:G26)</f>
-        <v>957</v>
+        <v>994.5</v>
       </c>
     </row>
     <row r="35" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F35" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G35" s="12">
+      <c r="G35" s="18">
         <f>G34*19%</f>
-        <v>181.83</v>
+        <v>188.95500000000001</v>
       </c>
     </row>
     <row r="36" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F36" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="12">
+      <c r="G36" s="18">
         <f>SUM(G34:G35)</f>
-        <v>1138.83</v>
+        <v>1183.4549999999999</v>
       </c>
     </row>
     <row r="37" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
feat: (#14, #19) Excelsteuerung flexibel
</commit_message>
<xml_diff>
--- a/TestRechnung.xlsx
+++ b/TestRechnung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herbe\Documents\Development\excel2zugferd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86400CEB-223D-4EB6-8303-DF45461313B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E01B8AB-C28E-4BE6-A572-0DB0C9D462E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="276" yWindow="1500" windowWidth="20436" windowHeight="13992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="816" windowWidth="18348" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="37">
   <si>
     <t>An:</t>
   </si>
@@ -132,6 +132,18 @@
   </si>
   <si>
     <t>Anfahrt dazu</t>
+  </si>
+  <si>
+    <t>Rechnungsdatum:</t>
+  </si>
+  <si>
+    <t>(optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rechnungsdatum: </t>
+  </si>
+  <si>
+    <t>Das Datum für die Rechnung; Es wird nach "Rechnungsdatum:" gesucht.</t>
   </si>
 </sst>
 </file>
@@ -559,10 +571,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -588,55 +600,63 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F12" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F13" s="12" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G15" s="15" t="s">
         <v>28</v>
       </c>
     </row>
@@ -651,10 +671,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -701,65 +721,50 @@
         <v>20240001</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="8" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="7">
+        <v>45321</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
-      <c r="B10" s="7">
-        <v>45292</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="12">
-        <f t="shared" ref="F10:F20" si="0">IF(E10="10 Min.",22,75)</f>
-        <v>22</v>
-      </c>
-      <c r="G10" s="12">
-        <f t="shared" ref="G10:G20" si="1">D10*F10</f>
-        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <f t="shared" ref="A11:A19" si="2">A10+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="7">
-        <v>45293</v>
+        <v>45292</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6">
         <v>1</v>
@@ -768,21 +773,21 @@
         <v>9</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F11:F21" si="0">IF(E11="10 Min.",22,75)</f>
         <v>22</v>
       </c>
       <c r="G11" s="12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G11:G21" si="1">D11*F11</f>
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f t="shared" ref="A12:A20" si="2">A11+1</f>
+        <v>2</v>
       </c>
       <c r="B12" s="7">
-        <v>45294</v>
+        <v>45293</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -805,94 +810,94 @@
     <row r="13" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13" s="7">
         <v>45294</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F13" s="12">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="G13" s="12">
         <f t="shared" si="1"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="7">
-        <v>45295</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>19</v>
+        <v>45294</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
       </c>
       <c r="D14" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F14" s="12">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="G14" s="12">
         <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="7">
-        <v>45296</v>
+        <v>45295</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="6">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F15" s="12">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="G15" s="12">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="7">
-        <v>45302</v>
+        <v>45296</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="6">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -903,112 +908,134 @@
       </c>
       <c r="G16" s="12">
         <f t="shared" si="1"/>
-        <v>525</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="7">
         <v>45302</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F17" s="12">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>75</v>
       </c>
       <c r="G17" s="12">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>525</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="B18" s="7">
+        <v>45302</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="7">
-        <v>45309</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
-      </c>
-      <c r="E18" t="s">
-        <v>10</v>
-      </c>
       <c r="F18" s="12">
         <f t="shared" si="0"/>
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="G18" s="12">
         <f t="shared" si="1"/>
-        <v>75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" s="7">
         <v>45309</v>
       </c>
       <c r="C19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="G19" s="12">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="B20" s="7">
+        <v>45309</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="6">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D20" s="6">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="12">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="G19" s="12">
-        <f t="shared" si="1"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
+      <c r="F20" s="12">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="G20" s="12">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
         <v>11</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D21" s="17">
         <v>0.5</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="12">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G21" s="10">
         <f t="shared" si="1"/>
         <v>37.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E21" s="8"/>
-      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E22" s="8"/>
@@ -1059,35 +1086,39 @@
       <c r="F33" s="12"/>
     </row>
     <row r="34" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F34" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="12">
-        <f>SUM(G10:G26)</f>
-        <v>994.5</v>
-      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="12"/>
     </row>
     <row r="35" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="18">
-        <f>G34*19%</f>
-        <v>188.95500000000001</v>
+        <v>8</v>
+      </c>
+      <c r="G35" s="12">
+        <f>SUM(G11:G27)</f>
+        <v>994.5</v>
       </c>
     </row>
     <row r="36" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F36" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="18">
+        <f>G35*19%</f>
+        <v>188.95500000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F37" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G36" s="18">
-        <f>SUM(G34:G35)</f>
+      <c r="G37" s="18">
+        <f>SUM(G35:G36)</f>
         <v>1183.4549999999999</v>
       </c>
     </row>
-    <row r="37" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E37" s="8"/>
-      <c r="F37" s="12"/>
+    <row r="38" spans="5:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="8"/>
+      <c r="F38" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>